<commit_message>
Another cleanup. Added header webelements, locators and builder. Added IE11 support
</commit_message>
<xml_diff>
--- a/Execon_-_TMO_SML_main.xlsx
+++ b/Execon_-_TMO_SML_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\TMO.R.AutomatedTestsSML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005FE829-B5C9-4538-ADE9-DC8612D358A8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2C205D-5C77-4253-8DAD-ACF20C44762F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17910" windowHeight="5850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Parametr</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>TS01</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>Internet explorer driver path</t>
+  </si>
+  <si>
+    <t>IEDriverServer.exe</t>
   </si>
 </sst>
 </file>
@@ -600,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,211 +699,227 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="A26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>443</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>46</v>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>443</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="7"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>60</v>
       </c>
     </row>
@@ -904,9 +929,9 @@
     <mergeCell ref="A9:B9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B30" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B36" r:id="rId3" xr:uid="{B8DA02D3-87C5-453F-BF59-D88FF5CAEE7E}"/>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B32" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B38" r:id="rId3" xr:uid="{B8DA02D3-87C5-453F-BF59-D88FF5CAEE7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>